<commit_message>
Data cleaning and preparation fix
</commit_message>
<xml_diff>
--- a/dataset/01_raw_home_loan_approval.xlsx
+++ b/dataset/01_raw_home_loan_approval.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Huawei\OneDrive - Universiti Malaya\Desktop\SEMESTER 7\WIE3010_Data-Visuals\loan-approval-data-visualization\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://365umedumy-my.sharepoint.com/personal/u2102810_siswa365_um_edu_my/Documents/Desktop/SEMESTER 7/WIE3010_Data-Visuals/loan-approval-data-visualization/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70F948C2-5143-47DD-805B-D7E6EEC9D6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{70F948C2-5143-47DD-805B-D7E6EEC9D6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C27562B5-4EBD-40A0-BB4E-6DDA3D33738A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{35BBE2C8-6948-49C7-89F1-6015018D725E}"/>
   </bookViews>
   <sheets>
-    <sheet name="raw_home_loan_approval_2" sheetId="1" r:id="rId1"/>
+    <sheet name="raw_home_loan_approval" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -2799,7 +2799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC5F294-B4E1-4650-A790-E0BDFE3DE06F}">
   <dimension ref="A1:M615"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>